<commit_message>
Updated the progress in Excel
</commit_message>
<xml_diff>
--- a/Excel workplan.xlsx
+++ b/Excel workplan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NTU\Y2S1\CZ2006\Project_GitHub\TeamNugget\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CZ2006\Teamnugget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB58C606-BF33-47C4-BD67-0A2C18919DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F1A182-9B63-48E2-8296-93D29D78F6EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{EEBB826D-426D-45D7-B67A-475D8D46EA92}"/>
+    <workbookView xWindow="10968" yWindow="2724" windowWidth="21180" windowHeight="9240" xr2:uid="{EEBB826D-426D-45D7-B67A-475D8D46EA92}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
   <si>
     <t>S/N</t>
   </si>
@@ -572,21 +572,21 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
     <col min="7" max="7" width="51" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -609,7 +609,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -626,7 +626,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -641,7 +641,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -656,7 +656,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -673,7 +673,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -688,7 +688,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -703,7 +703,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -724,7 +724,7 @@
       </c>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -740,10 +740,12 @@
       <c r="E9" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -759,10 +761,12 @@
       <c r="E10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -778,10 +782,12 @@
       <c r="E11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="F11" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -797,10 +803,12 @@
       <c r="E12" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="3"/>
+      <c r="F12" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -819,7 +827,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -838,7 +846,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -857,7 +865,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -874,7 +882,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -891,7 +899,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -910,7 +918,7 @@
       </c>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -931,7 +939,7 @@
       </c>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -948,7 +956,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -963,7 +971,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -978,7 +986,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>

</xml_diff>